<commit_message>
- 接続ボタン追加 - version表示追加 - SerialDevice・SerialManager削除 - remoconRoboLib・quadCrawlerソース追加 - 不要ファイル削除
</commit_message>
<xml_diff>
--- a/src/locale/locale.xlsx
+++ b/src/locale/locale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n-tom\Desktop\リモコンロボ\arduinoForMBlock\locale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n-tom\Desktop\FDrobot\mBlock\src\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="1627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="1555">
   <si>
     <t>ja</t>
   </si>
@@ -3051,12 +3051,6 @@
     <t>新しい変数</t>
   </si>
   <si>
-    <t>Eighth</t>
-  </si>
-  <si>
-    <t>8分音符</t>
-  </si>
-  <si>
     <t>Share to Scratch Website</t>
   </si>
   <si>
@@ -3252,12 +3246,6 @@
     <t>楽器</t>
   </si>
   <si>
-    <t>Quarter</t>
-  </si>
-  <si>
-    <t>4分音符</t>
-  </si>
-  <si>
     <t>rotation style:</t>
   </si>
   <si>
@@ -3330,12 +3318,6 @@
     <t>Bluetoothが見つかりません</t>
   </si>
   <si>
-    <t>Half</t>
-  </si>
-  <si>
-    <t>2分音符</t>
-  </si>
-  <si>
     <t>show list %m.list</t>
   </si>
   <si>
@@ -3576,12 +3558,6 @@
     <t>ソースを確認する</t>
   </si>
   <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>倍全音符</t>
-  </si>
-  <si>
     <t>Wooden Flute</t>
   </si>
   <si>
@@ -3744,12 +3720,6 @@
     <t>背景を %m.backdrop にする</t>
   </si>
   <si>
-    <t>Whole</t>
-  </si>
-  <si>
-    <t>全音符</t>
-  </si>
-  <si>
     <t>Choir</t>
   </si>
   <si>
@@ -4062,24 +4032,6 @@
     <t>light intensity</t>
   </si>
   <si>
-    <t>turn left</t>
-  </si>
-  <si>
-    <t>turn right</t>
-  </si>
-  <si>
-    <t>run backward</t>
-  </si>
-  <si>
-    <t>後</t>
-  </si>
-  <si>
-    <t>run forward</t>
-  </si>
-  <si>
-    <t>前</t>
-  </si>
-  <si>
     <t>pressed</t>
   </si>
   <si>
@@ -4164,12 +4116,6 @@
     <t>焦点を合わせない</t>
   </si>
   <si>
-    <t>set motor%d.motorPort speed %d.motorvalue</t>
-  </si>
-  <si>
-    <t>モーター %d.motorPort の速さを %d.motorvalue にする</t>
-  </si>
-  <si>
     <t>humidity</t>
   </si>
   <si>
@@ -4182,24 +4128,6 @@
     <t>温度</t>
   </si>
   <si>
-    <t>stop tone</t>
-  </si>
-  <si>
-    <t>音を止める</t>
-  </si>
-  <si>
-    <t>read digital pin %n</t>
-  </si>
-  <si>
-    <t>デジタルピン %n</t>
-  </si>
-  <si>
-    <t>set digital pin %n output as %d.digital</t>
-  </si>
-  <si>
-    <t>デジタルピン %n の出力を %d.digital にする</t>
-  </si>
-  <si>
     <t>sound on board</t>
   </si>
   <si>
@@ -4266,12 +4194,6 @@
     <t>バランスモード</t>
   </si>
   <si>
-    <t>set servo %d.servoSlot angle %d.servovalue</t>
-  </si>
-  <si>
-    <t>サーボ %d.servoSlot の角度を %d.servovalue にする</t>
-  </si>
-  <si>
     <t>no serial port</t>
   </si>
   <si>
@@ -4626,12 +4548,6 @@
     <t>ドライバをインストール</t>
   </si>
   <si>
-    <t>remote pressed</t>
-  </si>
-  <si>
-    <t>リモコンボタンが押された</t>
-  </si>
-  <si>
     <t>Educators' Content</t>
   </si>
   <si>
@@ -4644,9 +4560,6 @@
     <t>真ん中</t>
   </si>
   <si>
-    <t>LEDを %d.onoff</t>
-  </si>
-  <si>
     <t>ロボットをPC通信モードに設定</t>
   </si>
   <si>
@@ -4657,105 +4570,6 @@
   </si>
   <si>
     <t>はい</t>
-  </si>
-  <si>
-    <t>play tone on note %d.noteJ1 beat %d.beats</t>
-  </si>
-  <si>
-    <t>play tone on note %d.noteJ2 beat %d.beats</t>
-  </si>
-  <si>
-    <t>play tone on note %d.noteJ3 beat %d.beats</t>
-  </si>
-  <si>
-    <t>%d.noteJ1 を %d.beats 鳴らす</t>
-  </si>
-  <si>
-    <t>%d.noteJ2 を %d.beats 鳴らす</t>
-  </si>
-  <si>
-    <t>%d.noteJ3 を %d.beats 鳴らす</t>
-  </si>
-  <si>
-    <t>%d.direction at speed %d.speedvalue</t>
-  </si>
-  <si>
-    <t>%d.direction 向きに %d.speedvalue の速さで動かす</t>
-  </si>
-  <si>
-    <t>calibration right %n</t>
-  </si>
-  <si>
-    <t>read calibration</t>
-  </si>
-  <si>
-    <t>set calibration %n</t>
-  </si>
-  <si>
-    <t>calibration left %n</t>
-  </si>
-  <si>
-    <t>補正データ</t>
-  </si>
-  <si>
-    <t>ir remote %d.ircode pressed</t>
-  </si>
-  <si>
-    <t>押されたのが %d.ircode のボタン</t>
-  </si>
-  <si>
-    <t>analog remote %d.ircodeA pressed</t>
-  </si>
-  <si>
-    <t>get remote X</t>
-  </si>
-  <si>
-    <t>get remote Y</t>
-  </si>
-  <si>
-    <t>押されたのがアナログ %d.ircodeA のボタン</t>
-  </si>
-  <si>
-    <t>アナログXの値</t>
-  </si>
-  <si>
-    <t>アナログYの値</t>
-  </si>
-  <si>
-    <t>set digital pin A%n output as %d.digital</t>
-  </si>
-  <si>
-    <t>デジタルピン A%n の出力を %d.digital にする</t>
-  </si>
-  <si>
-    <t>read analog pin A%n</t>
-  </si>
-  <si>
-    <t>read digital pin A%n</t>
-  </si>
-  <si>
-    <t>デジタルピン A%n</t>
-  </si>
-  <si>
-    <t>右に%n 補正</t>
-  </si>
-  <si>
-    <t>左に%n 補正</t>
-  </si>
-  <si>
-    <t>補正データを%n に設定</t>
-  </si>
-  <si>
-    <t>Play MP3 track %n with loop %d.onoff</t>
-  </si>
-  <si>
-    <t>Stop MP3</t>
-  </si>
-  <si>
-    <t>MP3を止める</t>
-  </si>
-  <si>
-    <t>MP3の%n 曲目をループ%d.onoff で再生</t>
   </si>
   <si>
     <t>×動き</t>
@@ -4874,15 +4688,6 @@
     <t>プログラム開始</t>
   </si>
   <si>
-    <t>set LED %d.onoff</t>
-  </si>
-  <si>
-    <t>play tone on note %d.note beat %d.beats</t>
-  </si>
-  <si>
-    <t>%d.note を %d.beats 鳴らす</t>
-  </si>
-  <si>
     <t>接続中</t>
   </si>
   <si>
@@ -4899,30 +4704,6 @@
   </si>
   <si>
     <t>Connect to Robot</t>
-  </si>
-  <si>
-    <t>rotate left</t>
-  </si>
-  <si>
-    <t>左旋回</t>
-  </si>
-  <si>
-    <t>rotate right</t>
-  </si>
-  <si>
-    <t>右旋回</t>
-  </si>
-  <si>
-    <t>アナログピン A%n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>アナログピン A%n の %n 回平均</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read analog pin A%n average %n times</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6830,10 +6611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B854"/>
+  <dimension ref="A1:B843"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A824" workbookViewId="0">
-      <selection activeCell="B843" sqref="B843"/>
+    <sheetView tabSelected="1" topLeftCell="A573" workbookViewId="0">
+      <selection activeCell="A588" sqref="A588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4"/>
@@ -6860,7 +6641,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1579</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6868,7 +6649,7 @@
         <v>620</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1580</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6876,7 +6657,7 @@
         <v>421</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1581</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6884,7 +6665,7 @@
         <v>268</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1582</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6892,7 +6673,7 @@
         <v>600</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1583</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6900,7 +6681,7 @@
         <v>197</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1584</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6916,7 +6697,7 @@
         <v>653</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1585</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -7001,10 +6782,10 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -7017,10 +6798,10 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -7161,7 +6942,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>1212</v>
+        <v>1204</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>11</v>
@@ -7193,18 +6974,18 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>1239</v>
+        <v>1231</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>1240</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>1260</v>
+        <v>1250</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>1240</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -7337,18 +7118,18 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -7425,10 +7206,10 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2" t="s">
-        <v>1215</v>
+        <v>1207</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>1216</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -7452,7 +7233,7 @@
         <v>385</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>1586</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -7473,15 +7254,15 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2" t="s">
-        <v>1236</v>
+        <v>1228</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>631</v>
@@ -7529,10 +7310,10 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2" t="s">
-        <v>1181</v>
+        <v>1175</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>1182</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -7601,7 +7382,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2" t="s">
-        <v>1587</v>
+        <v>1525</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>914</v>
@@ -7721,10 +7502,10 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -7841,10 +7622,10 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2" t="s">
-        <v>1203</v>
+        <v>1195</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>1204</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -7889,10 +7670,10 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="2" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -8105,10 +7886,10 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="2" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -8129,26 +7910,26 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>1233</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>1198</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2" t="s">
-        <v>1201</v>
+        <v>1193</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>1202</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -8233,10 +8014,10 @@
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2" t="s">
-        <v>1531</v>
+        <v>1505</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>1532</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -8273,34 +8054,34 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -8340,7 +8121,7 @@
         <v>7</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>1534</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -8684,7 +8465,7 @@
         <v>122</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>1588</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -8740,7 +8521,7 @@
         <v>139</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>1543</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -9388,7 +9169,7 @@
         <v>399</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>1533</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -9401,7 +9182,7 @@
     </row>
     <row r="321" spans="1:2">
       <c r="A321" s="2" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B321" s="5" t="s">
         <v>422</v>
@@ -9412,7 +9193,7 @@
         <v>404</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>1589</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -9604,7 +9385,7 @@
         <v>470</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>1538</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -10540,7 +10321,7 @@
         <v>813</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>1539</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="464" spans="1:2">
@@ -10564,7 +10345,7 @@
         <v>820</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>1539</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="467" spans="1:2">
@@ -10620,7 +10401,7 @@
         <v>835</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>1539</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="474" spans="1:2">
@@ -11076,7 +10857,7 @@
         <v>972</v>
       </c>
       <c r="B530" s="5" t="s">
-        <v>1614</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="531" spans="1:2">
@@ -11209,31 +10990,31 @@
     </row>
     <row r="547" spans="1:2">
       <c r="A547" s="2" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B547" s="5" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="548" spans="1:2">
       <c r="A548" s="2" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B548" s="5" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="549" spans="1:2">
       <c r="A549" s="2" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B549" s="5" t="s">
-        <v>1218</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="550" spans="1:2">
       <c r="A550" s="2" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B550" s="5" t="s">
         <v>136</v>
@@ -11241,42 +11022,42 @@
     </row>
     <row r="551" spans="1:2">
       <c r="A551" s="2" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B551" s="5" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="552" spans="1:2">
       <c r="A552" s="2" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B552" s="5" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="553" spans="1:2">
       <c r="A553" s="2" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B553" s="5" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="554" spans="1:2">
       <c r="A554" s="2" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B554" s="5" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="555" spans="1:2">
       <c r="A555" s="2" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B555" s="5" t="s">
-        <v>1590</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="556" spans="1:2">
@@ -11289,79 +11070,79 @@
     </row>
     <row r="557" spans="1:2">
       <c r="A557" s="2" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B557" s="5" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="558" spans="1:2">
       <c r="A558" s="2" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B558" s="5" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="559" spans="1:2">
       <c r="A559" s="2" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B559" s="5" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="560" spans="1:2">
       <c r="A560" s="2" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B560" s="5" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="561" spans="1:2">
       <c r="A561" s="2" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="562" spans="1:2">
       <c r="A562" s="2" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B562" s="5" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="563" spans="1:2">
       <c r="A563" s="2" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="B563" s="5" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="564" spans="1:2">
       <c r="A564" s="2" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B564" s="5" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="565" spans="1:2">
       <c r="A565" s="2" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B565" s="5" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="566" spans="1:2">
       <c r="A566" s="2" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B566" s="5" t="s">
         <v>415</v>
@@ -11369,690 +11150,690 @@
     </row>
     <row r="567" spans="1:2">
       <c r="A567" s="2" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B567" s="5" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="568" spans="1:2">
       <c r="A568" s="2" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B568" s="5" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="569" spans="1:2">
       <c r="A569" s="2" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B569" s="5" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="570" spans="1:2">
       <c r="A570" s="2" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B570" s="5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="571" spans="1:2">
       <c r="A571" s="2" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B571" s="5" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="572" spans="1:2">
       <c r="A572" s="2" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="B572" s="5" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="573" spans="1:2">
       <c r="A573" s="2" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B573" s="5" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="574" spans="1:2">
       <c r="A574" s="2" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B574" s="5" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="575" spans="1:2">
       <c r="A575" s="2" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="B575" s="5" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="576" spans="1:2">
       <c r="A576" s="2" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="B576" s="5" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="577" spans="1:2">
       <c r="A577" s="2" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="B577" s="5" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="578" spans="1:2">
       <c r="A578" s="2" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="B578" s="5" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="579" spans="1:2">
       <c r="A579" s="2" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="B579" s="5" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="580" spans="1:2">
       <c r="A580" s="2" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="B580" s="5" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="581" spans="1:2">
       <c r="A581" s="2" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="B581" s="5" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="582" spans="1:2">
       <c r="A582" s="2" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="B582" s="5" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="583" spans="1:2">
       <c r="A583" s="2" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B583" s="2" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="584" spans="1:2">
       <c r="A584" s="2" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="585" spans="1:2">
       <c r="A585" s="2" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="B585" s="5" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="586" spans="1:2">
       <c r="A586" s="2" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="B586" s="5" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="587" spans="1:2">
       <c r="A587" s="2" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="B587" s="5" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="588" spans="1:2">
       <c r="A588" s="2" t="s">
-        <v>1077</v>
+        <v>1101</v>
       </c>
       <c r="B588" s="5" t="s">
-        <v>1078</v>
+        <v>364</v>
       </c>
     </row>
     <row r="589" spans="1:2">
       <c r="A589" s="2" t="s">
-        <v>1010</v>
+        <v>1102</v>
       </c>
       <c r="B589" s="5" t="s">
-        <v>1011</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="590" spans="1:2">
       <c r="A590" s="2" t="s">
-        <v>1241</v>
+        <v>1104</v>
       </c>
       <c r="B590" s="5" t="s">
-        <v>1242</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="591" spans="1:2">
       <c r="A591" s="2" t="s">
-        <v>1185</v>
+        <v>1106</v>
       </c>
       <c r="B591" s="5" t="s">
-        <v>1186</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="592" spans="1:2">
       <c r="A592" s="2" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="B592" s="5" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="593" spans="1:2">
       <c r="A593" s="2" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="B593" s="5" t="s">
-        <v>364</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="594" spans="1:2">
       <c r="A594" s="2" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="B594" s="5" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="595" spans="1:2">
       <c r="A595" s="2" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="B595" s="5" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="596" spans="1:2">
       <c r="A596" s="2" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="B596" s="5" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="597" spans="1:2">
       <c r="A597" s="2" t="s">
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="B597" s="5" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="598" spans="1:2">
       <c r="A598" s="2" t="s">
-        <v>1116</v>
+        <v>1119</v>
       </c>
       <c r="B598" s="5" t="s">
-        <v>1064</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="599" spans="1:2">
       <c r="A599" s="2" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
       <c r="B599" s="5" t="s">
-        <v>1118</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="600" spans="1:2">
       <c r="A600" s="2" t="s">
-        <v>1119</v>
+        <v>1125</v>
       </c>
       <c r="B600" s="5" t="s">
-        <v>1120</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="601" spans="1:2">
       <c r="A601" s="2" t="s">
-        <v>1121</v>
+        <v>1127</v>
       </c>
       <c r="B601" s="5" t="s">
-        <v>1122</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="602" spans="1:2">
       <c r="A602" s="2" t="s">
-        <v>1123</v>
+        <v>1131</v>
       </c>
       <c r="B602" s="5" t="s">
-        <v>1124</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="603" spans="1:2">
       <c r="A603" s="2" t="s">
-        <v>1125</v>
+        <v>1133</v>
       </c>
       <c r="B603" s="5" t="s">
-        <v>1126</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="604" spans="1:2">
       <c r="A604" s="2" t="s">
-        <v>1127</v>
+        <v>1135</v>
       </c>
       <c r="B604" s="5" t="s">
-        <v>1128</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="605" spans="1:2">
       <c r="A605" s="2" t="s">
-        <v>1131</v>
+        <v>1137</v>
       </c>
       <c r="B605" s="5" t="s">
-        <v>1132</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="606" spans="1:2">
       <c r="A606" s="2" t="s">
-        <v>1133</v>
+        <v>1139</v>
       </c>
       <c r="B606" s="5" t="s">
-        <v>1134</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="607" spans="1:2">
       <c r="A607" s="2" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="B607" s="5" t="s">
-        <v>1138</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="608" spans="1:2">
       <c r="A608" s="2" t="s">
-        <v>1139</v>
+        <v>1145</v>
       </c>
       <c r="B608" s="5" t="s">
-        <v>1140</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="609" spans="1:2">
       <c r="A609" s="2" t="s">
-        <v>1141</v>
+        <v>1147</v>
       </c>
       <c r="B609" s="5" t="s">
-        <v>1142</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="610" spans="1:2">
       <c r="A610" s="2" t="s">
-        <v>1143</v>
+        <v>1151</v>
       </c>
       <c r="B610" s="5" t="s">
-        <v>1144</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="611" spans="1:2">
       <c r="A611" s="2" t="s">
-        <v>1145</v>
+        <v>1153</v>
       </c>
       <c r="B611" s="5" t="s">
-        <v>1146</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="612" spans="1:2">
       <c r="A612" s="2" t="s">
-        <v>1147</v>
+        <v>1155</v>
       </c>
       <c r="B612" s="5" t="s">
-        <v>1148</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="613" spans="1:2">
       <c r="A613" s="2" t="s">
-        <v>1151</v>
+        <v>1157</v>
       </c>
       <c r="B613" s="5" t="s">
-        <v>1152</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="614" spans="1:2">
       <c r="A614" s="2" t="s">
-        <v>1153</v>
+        <v>1205</v>
       </c>
       <c r="B614" s="5" t="s">
-        <v>1154</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="615" spans="1:2">
       <c r="A615" s="2" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="B615" s="5" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="616" spans="1:2">
       <c r="A616" s="2" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="B616" s="5" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="617" spans="1:2">
       <c r="A617" s="2" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
       <c r="B617" s="5" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="618" spans="1:2">
       <c r="A618" s="2" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="B618" s="5" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="619" spans="1:2">
       <c r="A619" s="2" t="s">
-        <v>1213</v>
+        <v>1167</v>
       </c>
       <c r="B619" s="5" t="s">
-        <v>1214</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="620" spans="1:2">
       <c r="A620" s="2" t="s">
-        <v>1165</v>
+        <v>1169</v>
       </c>
       <c r="B620" s="5" t="s">
-        <v>1166</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="621" spans="1:2">
       <c r="A621" s="2" t="s">
-        <v>1167</v>
+        <v>1171</v>
       </c>
       <c r="B621" s="5" t="s">
-        <v>1168</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="622" spans="1:2">
       <c r="A622" s="2" t="s">
-        <v>1169</v>
+        <v>1173</v>
       </c>
       <c r="B622" s="5" t="s">
-        <v>1170</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="623" spans="1:2">
       <c r="A623" s="2" t="s">
-        <v>1171</v>
+        <v>1177</v>
       </c>
       <c r="B623" s="5" t="s">
-        <v>1172</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="624" spans="1:2">
       <c r="A624" s="2" t="s">
-        <v>1173</v>
+        <v>1179</v>
       </c>
       <c r="B624" s="5" t="s">
-        <v>1174</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="625" spans="1:2">
       <c r="A625" s="2" t="s">
-        <v>1175</v>
+        <v>1183</v>
       </c>
       <c r="B625" s="5" t="s">
-        <v>1176</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="626" spans="1:2">
       <c r="A626" s="2" t="s">
-        <v>1177</v>
+        <v>1185</v>
       </c>
       <c r="B626" s="5" t="s">
-        <v>1178</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="627" spans="1:2">
       <c r="A627" s="2" t="s">
-        <v>1179</v>
+        <v>1187</v>
       </c>
       <c r="B627" s="5" t="s">
-        <v>1180</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="628" spans="1:2">
       <c r="A628" s="2" t="s">
-        <v>1183</v>
+        <v>1191</v>
       </c>
       <c r="B628" s="5" t="s">
-        <v>1184</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="629" spans="1:2">
       <c r="A629" s="2" t="s">
-        <v>1187</v>
+        <v>1197</v>
       </c>
       <c r="B629" s="5" t="s">
-        <v>1188</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="630" spans="1:2">
       <c r="A630" s="2" t="s">
-        <v>1191</v>
+        <v>1198</v>
       </c>
       <c r="B630" s="5" t="s">
-        <v>1192</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="631" spans="1:2">
       <c r="A631" s="2" t="s">
-        <v>1193</v>
+        <v>1200</v>
       </c>
       <c r="B631" s="5" t="s">
-        <v>1194</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="632" spans="1:2">
       <c r="A632" s="2" t="s">
-        <v>1195</v>
+        <v>1202</v>
       </c>
       <c r="B632" s="5" t="s">
-        <v>1196</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="633" spans="1:2">
       <c r="A633" s="2" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B633" s="5" t="s">
-        <v>1200</v>
+        <v>1209</v>
+      </c>
+      <c r="B633" s="7" t="s">
+        <v>1210</v>
       </c>
     </row>
     <row r="634" spans="1:2">
       <c r="A634" s="2" t="s">
-        <v>1205</v>
+        <v>1211</v>
       </c>
       <c r="B634" s="5" t="s">
-        <v>1542</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="635" spans="1:2">
       <c r="A635" s="2" t="s">
-        <v>1206</v>
+        <v>1213</v>
       </c>
       <c r="B635" s="5" t="s">
-        <v>1207</v>
+        <v>109</v>
       </c>
     </row>
     <row r="636" spans="1:2">
       <c r="A636" s="2" t="s">
-        <v>1208</v>
+        <v>1214</v>
       </c>
       <c r="B636" s="5" t="s">
-        <v>1209</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="637" spans="1:2">
       <c r="A637" s="2" t="s">
-        <v>1210</v>
+        <v>1216</v>
       </c>
       <c r="B637" s="5" t="s">
-        <v>1211</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="638" spans="1:2">
       <c r="A638" s="2" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B638" s="7" t="s">
         <v>1218</v>
+      </c>
+      <c r="B638" s="5" t="s">
+        <v>1219</v>
       </c>
     </row>
     <row r="639" spans="1:2">
       <c r="A639" s="2" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B639" s="5" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="640" spans="1:2">
       <c r="A640" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="B640" s="5" t="s">
-        <v>109</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="641" spans="1:2">
       <c r="A641" s="2" t="s">
-        <v>1222</v>
+        <v>1226</v>
       </c>
       <c r="B641" s="5" t="s">
-        <v>1223</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="642" spans="1:2">
       <c r="A642" s="2" t="s">
-        <v>1224</v>
+        <v>1229</v>
       </c>
       <c r="B642" s="5" t="s">
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="643" spans="1:2">
       <c r="A643" s="2" t="s">
-        <v>1226</v>
+        <v>1233</v>
       </c>
       <c r="B643" s="5" t="s">
-        <v>1227</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="644" spans="1:2">
       <c r="A644" s="2" t="s">
-        <v>1228</v>
+        <v>1235</v>
       </c>
       <c r="B644" s="5" t="s">
-        <v>1229</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="645" spans="1:2">
       <c r="A645" s="2" t="s">
-        <v>1230</v>
+        <v>1236</v>
       </c>
       <c r="B645" s="5" t="s">
-        <v>1231</v>
+        <v>950</v>
       </c>
     </row>
     <row r="646" spans="1:2">
       <c r="A646" s="2" t="s">
-        <v>1234</v>
+        <v>1237</v>
       </c>
       <c r="B646" s="5" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="647" spans="1:2">
       <c r="A647" s="2" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="B647" s="5" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="648" spans="1:2">
       <c r="A648" s="2" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B648" s="5" t="s">
-        <v>1244</v>
+        <v>199</v>
       </c>
     </row>
     <row r="649" spans="1:2">
       <c r="A649" s="2" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="B649" s="5" t="s">
-        <v>1591</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="650" spans="1:2">
       <c r="A650" s="2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="B650" s="5" t="s">
-        <v>950</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="651" spans="1:2">
       <c r="A651" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B651" s="5" t="s">
         <v>1247</v>
-      </c>
-      <c r="B651" s="5" t="s">
-        <v>1248</v>
       </c>
     </row>
     <row r="652" spans="1:2">
       <c r="A652" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B652" s="5" t="s">
         <v>1249</v>
-      </c>
-      <c r="B652" s="5" t="s">
-        <v>1250</v>
       </c>
     </row>
     <row r="653" spans="1:2">
@@ -12060,39 +11841,39 @@
         <v>1251</v>
       </c>
       <c r="B653" s="5" t="s">
-        <v>199</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="654" spans="1:2">
       <c r="A654" s="2" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="B654" s="5" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="655" spans="1:2">
       <c r="A655" s="2" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="B655" s="5" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="656" spans="1:2">
       <c r="A656" s="2" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="B656" s="5" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="657" spans="1:2">
       <c r="A657" s="2" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="B657" s="5" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="658" spans="1:2">
@@ -12147,48 +11928,48 @@
       <c r="A664" s="2" t="s">
         <v>1273</v>
       </c>
-      <c r="B664" s="5" t="s">
-        <v>1274</v>
+      <c r="B664" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="665" spans="1:2">
       <c r="A665" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B665" s="5" t="s">
         <v>1275</v>
-      </c>
-      <c r="B665" s="5" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="666" spans="1:2">
       <c r="A666" s="2" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B666" s="7" t="s">
         <v>1277</v>
-      </c>
-      <c r="B666" s="5" t="s">
-        <v>1278</v>
       </c>
     </row>
     <row r="667" spans="1:2">
       <c r="A667" s="2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B667" s="5" t="s">
         <v>1279</v>
-      </c>
-      <c r="B667" s="5" t="s">
-        <v>1280</v>
       </c>
     </row>
     <row r="668" spans="1:2">
       <c r="A668" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B668" s="5" t="s">
         <v>1281</v>
-      </c>
-      <c r="B668" s="5" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="669" spans="1:2">
       <c r="A669" s="2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B669" s="5" t="s">
         <v>1283</v>
-      </c>
-      <c r="B669" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="670" spans="1:2">
@@ -12203,56 +11984,56 @@
       <c r="A671" s="2" t="s">
         <v>1286</v>
       </c>
-      <c r="B671" s="7" t="s">
-        <v>1287</v>
+      <c r="B671" s="5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="672" spans="1:2">
       <c r="A672" s="2" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B672" s="5" t="s">
-        <v>1289</v>
+        <v>298</v>
       </c>
     </row>
     <row r="673" spans="1:2">
       <c r="A673" s="2" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B673" s="5" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="674" spans="1:2">
       <c r="A674" s="2" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="B674" s="5" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="675" spans="1:2">
       <c r="A675" s="2" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B675" s="5" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="676" spans="1:2">
       <c r="A676" s="2" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B676" s="5" t="s">
-        <v>169</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="677" spans="1:2">
       <c r="A677" s="2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B677" s="5" t="s">
         <v>1297</v>
-      </c>
-      <c r="B677" s="5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="678" spans="1:2">
@@ -12265,66 +12046,66 @@
     </row>
     <row r="679" spans="1:2">
       <c r="A679" s="2" t="s">
-        <v>1300</v>
+        <v>532</v>
       </c>
       <c r="B679" s="5" t="s">
-        <v>1301</v>
+        <v>533</v>
       </c>
     </row>
     <row r="680" spans="1:2">
       <c r="A680" s="2" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B680" s="5" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="681" spans="1:2">
       <c r="A681" s="2" t="s">
-        <v>1304</v>
+        <v>1332</v>
       </c>
       <c r="B681" s="5" t="s">
-        <v>1305</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="682" spans="1:2">
       <c r="A682" s="2" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="B682" s="5" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="683" spans="1:2">
       <c r="A683" s="2" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="B683" s="5" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="684" spans="1:2">
       <c r="A684" s="2" t="s">
-        <v>532</v>
+        <v>1306</v>
       </c>
       <c r="B684" s="5" t="s">
-        <v>533</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="685" spans="1:2">
       <c r="A685" s="2" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="B685" s="5" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="686" spans="1:2">
       <c r="A686" s="2" t="s">
-        <v>1342</v>
+        <v>1310</v>
       </c>
       <c r="B686" s="5" t="s">
-        <v>1343</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="687" spans="1:2">
@@ -12388,31 +12169,31 @@
         <v>1326</v>
       </c>
       <c r="B694" s="5" t="s">
-        <v>1327</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="695" spans="1:2">
       <c r="A695" s="2" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B695" s="5" t="s">
-        <v>1329</v>
+        <v>1327</v>
+      </c>
+      <c r="B695" s="7" t="s">
+        <v>1516</v>
       </c>
     </row>
     <row r="696" spans="1:2">
       <c r="A696" s="2" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B696" s="5" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="697" spans="1:2">
       <c r="A697" s="2" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B697" s="5" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="698" spans="1:2">
@@ -12428,7 +12209,7 @@
         <v>1336</v>
       </c>
       <c r="B699" s="5" t="s">
-        <v>1544</v>
+        <v>245</v>
       </c>
     </row>
     <row r="700" spans="1:2">
@@ -12436,203 +12217,203 @@
         <v>1337</v>
       </c>
       <c r="B700" s="7" t="s">
-        <v>1545</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="701" spans="1:2">
       <c r="A701" s="2" t="s">
-        <v>1338</v>
-      </c>
-      <c r="B701" s="5" t="s">
         <v>1339</v>
+      </c>
+      <c r="B701" s="7" t="s">
+        <v>1340</v>
       </c>
     </row>
     <row r="702" spans="1:2">
       <c r="A702" s="2" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B702" s="5" t="s">
         <v>1341</v>
+      </c>
+      <c r="B702" s="7" t="s">
+        <v>1342</v>
       </c>
     </row>
     <row r="703" spans="1:2">
       <c r="A703" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B703" s="7" t="s">
         <v>1344</v>
-      </c>
-      <c r="B703" s="5" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="704" spans="1:2">
       <c r="A704" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B704" s="7" t="s">
         <v>1346</v>
-      </c>
-      <c r="B704" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="705" spans="1:2">
       <c r="A705" s="2" t="s">
         <v>1347</v>
       </c>
-      <c r="B705" s="5" t="s">
-        <v>609</v>
+      <c r="B705" s="7" t="s">
+        <v>1348</v>
       </c>
     </row>
     <row r="706" spans="1:2">
       <c r="A706" s="2" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B706" s="5" t="s">
-        <v>554</v>
+        <v>1349</v>
+      </c>
+      <c r="B706" s="7" t="s">
+        <v>1350</v>
       </c>
     </row>
     <row r="707" spans="1:2">
       <c r="A707" s="2" t="s">
-        <v>1349</v>
-      </c>
-      <c r="B707" s="5" t="s">
-        <v>1350</v>
+        <v>1351</v>
+      </c>
+      <c r="B707" s="7" t="s">
+        <v>1352</v>
       </c>
     </row>
     <row r="708" spans="1:2">
       <c r="A708" s="2" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B708" s="5" t="s">
-        <v>1352</v>
+        <v>1353</v>
+      </c>
+      <c r="B708" s="7" t="s">
+        <v>1354</v>
       </c>
     </row>
     <row r="709" spans="1:2">
       <c r="A709" s="2" t="s">
-        <v>1620</v>
-      </c>
-      <c r="B709" s="5" t="s">
-        <v>1621</v>
+        <v>1355</v>
+      </c>
+      <c r="B709" s="7" t="s">
+        <v>1356</v>
       </c>
     </row>
     <row r="710" spans="1:2">
       <c r="A710" s="2" t="s">
-        <v>1622</v>
-      </c>
-      <c r="B710" s="5" t="s">
-        <v>1623</v>
+        <v>1357</v>
+      </c>
+      <c r="B710" s="7" t="s">
+        <v>1358</v>
       </c>
     </row>
     <row r="711" spans="1:2">
       <c r="A711" s="2" t="s">
-        <v>1353</v>
+        <v>1359</v>
       </c>
       <c r="B711" s="7" t="s">
-        <v>1354</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="712" spans="1:2">
-      <c r="A712" s="2" t="s">
-        <v>1355</v>
+      <c r="A712" s="3" t="s">
+        <v>1361</v>
       </c>
       <c r="B712" s="7" t="s">
-        <v>1356</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="713" spans="1:2">
-      <c r="A713" s="2" t="s">
-        <v>1357</v>
+      <c r="A713" s="3" t="s">
+        <v>1363</v>
       </c>
       <c r="B713" s="7" t="s">
-        <v>1358</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="714" spans="1:2">
-      <c r="A714" s="2" t="s">
-        <v>1359</v>
+      <c r="A714" s="3" t="s">
+        <v>1365</v>
       </c>
       <c r="B714" s="7" t="s">
-        <v>1360</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="715" spans="1:2">
-      <c r="A715" s="2" t="s">
-        <v>1361</v>
+      <c r="A715" s="3" t="s">
+        <v>1367</v>
       </c>
       <c r="B715" s="7" t="s">
-        <v>1362</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="716" spans="1:2">
-      <c r="A716" s="2" t="s">
-        <v>1363</v>
+      <c r="A716" s="3" t="s">
+        <v>1158</v>
       </c>
       <c r="B716" s="7" t="s">
-        <v>1364</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="717" spans="1:2">
-      <c r="A717" s="2" t="s">
-        <v>1365</v>
+      <c r="A717" s="3" t="s">
+        <v>1206</v>
       </c>
       <c r="B717" s="7" t="s">
-        <v>1366</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="718" spans="1:2">
-      <c r="A718" s="2" t="s">
-        <v>1367</v>
+      <c r="A718" s="3" t="s">
+        <v>1369</v>
       </c>
       <c r="B718" s="7" t="s">
-        <v>1368</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="719" spans="1:2">
-      <c r="A719" s="2" t="s">
-        <v>1369</v>
+      <c r="A719" s="3" t="s">
+        <v>1371</v>
       </c>
       <c r="B719" s="7" t="s">
-        <v>1370</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="720" spans="1:2">
-      <c r="A720" s="2" t="s">
-        <v>1371</v>
+      <c r="A720" s="3" t="s">
+        <v>1373</v>
       </c>
       <c r="B720" s="7" t="s">
-        <v>1372</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="721" spans="1:2">
-      <c r="A721" s="2" t="s">
-        <v>1373</v>
+      <c r="A721" s="3" t="s">
+        <v>1375</v>
       </c>
       <c r="B721" s="7" t="s">
-        <v>1374</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="722" spans="1:2">
-      <c r="A722" s="2" t="s">
-        <v>1375</v>
+      <c r="A722" s="3" t="s">
+        <v>1377</v>
       </c>
       <c r="B722" s="7" t="s">
-        <v>1376</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="723" spans="1:2">
       <c r="A723" s="3" t="s">
-        <v>1377</v>
+        <v>1379</v>
       </c>
       <c r="B723" s="7" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="724" spans="1:2">
-      <c r="A724" s="3" t="s">
-        <v>1379</v>
+      <c r="A724" s="2" t="s">
+        <v>1381</v>
       </c>
       <c r="B724" s="7" t="s">
-        <v>1380</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="725" spans="1:2">
-      <c r="A725" s="3" t="s">
+      <c r="A725" s="2" t="s">
         <v>1383</v>
       </c>
       <c r="B725" s="7" t="s">
@@ -12643,970 +12424,756 @@
       <c r="A726" s="3" t="s">
         <v>1385</v>
       </c>
-      <c r="B726" s="7" t="s">
+      <c r="B726" s="3" t="s">
         <v>1386</v>
       </c>
     </row>
     <row r="727" spans="1:2">
       <c r="A727" s="3" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B727" s="7" t="s">
-        <v>1164</v>
+        <v>1387</v>
+      </c>
+      <c r="B727" s="3" t="s">
+        <v>1388</v>
       </c>
     </row>
     <row r="728" spans="1:2">
       <c r="A728" s="3" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B728" s="7" t="s">
-        <v>1214</v>
+        <v>1389</v>
+      </c>
+      <c r="B728" s="3" t="s">
+        <v>1390</v>
       </c>
     </row>
     <row r="729" spans="1:2">
       <c r="A729" s="3" t="s">
-        <v>1393</v>
-      </c>
-      <c r="B729" s="7" t="s">
-        <v>1394</v>
+        <v>1391</v>
+      </c>
+      <c r="B729" s="3" t="s">
+        <v>1392</v>
       </c>
     </row>
     <row r="730" spans="1:2">
       <c r="A730" s="3" t="s">
-        <v>1395</v>
-      </c>
-      <c r="B730" s="7" t="s">
-        <v>1396</v>
+        <v>1393</v>
+      </c>
+      <c r="B730" s="3" t="s">
+        <v>1394</v>
       </c>
     </row>
     <row r="731" spans="1:2">
       <c r="A731" s="3" t="s">
-        <v>1397</v>
-      </c>
-      <c r="B731" s="7" t="s">
-        <v>1398</v>
+        <v>1395</v>
+      </c>
+      <c r="B731" s="3" t="s">
+        <v>1396</v>
       </c>
     </row>
     <row r="732" spans="1:2">
       <c r="A732" s="3" t="s">
-        <v>1399</v>
-      </c>
-      <c r="B732" s="7" t="s">
-        <v>1400</v>
+        <v>1397</v>
+      </c>
+      <c r="B732" s="3" t="s">
+        <v>1398</v>
       </c>
     </row>
     <row r="733" spans="1:2">
       <c r="A733" s="3" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B733" s="7" t="s">
-        <v>1402</v>
+        <v>1399</v>
+      </c>
+      <c r="B733" s="3" t="s">
+        <v>1400</v>
       </c>
     </row>
     <row r="734" spans="1:2">
       <c r="A734" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B734" s="3" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2">
+      <c r="A735" s="3" t="s">
         <v>1403</v>
       </c>
-      <c r="B734" s="7" t="s">
+      <c r="B735" s="3" t="s">
         <v>1404</v>
       </c>
     </row>
-    <row r="735" spans="1:2">
-      <c r="A735" s="2" t="s">
+    <row r="736" spans="1:2">
+      <c r="A736" s="3" t="s">
         <v>1405</v>
       </c>
-      <c r="B735" s="7" t="s">
+      <c r="B736" s="3" t="s">
         <v>1406</v>
-      </c>
-    </row>
-    <row r="736" spans="1:2">
-      <c r="A736" s="2" t="s">
-        <v>1407</v>
-      </c>
-      <c r="B736" s="7" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="737" spans="1:2">
       <c r="A737" s="3" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="B737" s="3" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="738" spans="1:2">
       <c r="A738" s="3" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="B738" s="3" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="739" spans="1:2">
       <c r="A739" s="3" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="B739" s="3" t="s">
-        <v>1414</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="740" spans="1:2">
       <c r="A740" s="3" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="B740" s="3" t="s">
-        <v>1418</v>
+        <v>922</v>
       </c>
     </row>
     <row r="741" spans="1:2">
       <c r="A741" s="3" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="B741" s="3" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="742" spans="1:2">
       <c r="A742" s="3" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
       <c r="B742" s="3" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="743" spans="1:2">
       <c r="A743" s="3" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="B743" s="3" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="744" spans="1:2">
       <c r="A744" s="3" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>1426</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="745" spans="1:2">
       <c r="A745" s="3" t="s">
-        <v>1427</v>
+        <v>1421</v>
       </c>
       <c r="B745" s="3" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="746" spans="1:2">
       <c r="A746" s="3" t="s">
-        <v>1429</v>
+        <v>1423</v>
       </c>
       <c r="B746" s="3" t="s">
-        <v>1430</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="747" spans="1:2">
       <c r="A747" s="3" t="s">
-        <v>1431</v>
+        <v>1425</v>
       </c>
       <c r="B747" s="3" t="s">
-        <v>1432</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="748" spans="1:2">
       <c r="A748" s="3" t="s">
-        <v>1433</v>
+        <v>1427</v>
       </c>
       <c r="B748" s="3" t="s">
-        <v>1434</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="749" spans="1:2">
       <c r="A749" s="3" t="s">
-        <v>1435</v>
+        <v>405</v>
       </c>
       <c r="B749" s="3" t="s">
-        <v>1436</v>
+        <v>406</v>
       </c>
     </row>
     <row r="750" spans="1:2">
       <c r="A750" s="3" t="s">
-        <v>1437</v>
+        <v>567</v>
       </c>
       <c r="B750" s="3" t="s">
-        <v>1034</v>
+        <v>568</v>
       </c>
     </row>
     <row r="751" spans="1:2">
       <c r="A751" s="3" t="s">
-        <v>1438</v>
+        <v>1429</v>
       </c>
       <c r="B751" s="3" t="s">
-        <v>922</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="752" spans="1:2">
       <c r="A752" s="3" t="s">
-        <v>1439</v>
+        <v>1431</v>
       </c>
       <c r="B752" s="3" t="s">
-        <v>1440</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="753" spans="1:2">
       <c r="A753" s="3" t="s">
-        <v>1441</v>
+        <v>1433</v>
       </c>
       <c r="B753" s="3" t="s">
-        <v>1442</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="754" spans="1:2">
       <c r="A754" s="3" t="s">
-        <v>1443</v>
+        <v>1435</v>
       </c>
       <c r="B754" s="3" t="s">
-        <v>1444</v>
+        <v>682</v>
       </c>
     </row>
     <row r="755" spans="1:2">
       <c r="A755" s="3" t="s">
-        <v>1445</v>
+        <v>1436</v>
       </c>
       <c r="B755" s="3" t="s">
-        <v>1446</v>
+        <v>406</v>
       </c>
     </row>
     <row r="756" spans="1:2">
       <c r="A756" s="3" t="s">
-        <v>1447</v>
+        <v>1437</v>
       </c>
       <c r="B756" s="3" t="s">
-        <v>1448</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="757" spans="1:2">
       <c r="A757" s="3" t="s">
-        <v>1449</v>
+        <v>1439</v>
       </c>
       <c r="B757" s="3" t="s">
-        <v>1450</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="758" spans="1:2">
       <c r="A758" s="3" t="s">
-        <v>1451</v>
+        <v>1441</v>
       </c>
       <c r="B758" s="3" t="s">
-        <v>1452</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="759" spans="1:2">
       <c r="A759" s="3" t="s">
-        <v>1453</v>
+        <v>1442</v>
       </c>
       <c r="B759" s="3" t="s">
-        <v>1454</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="760" spans="1:2">
       <c r="A760" s="3" t="s">
-        <v>405</v>
+        <v>1443</v>
       </c>
       <c r="B760" s="3" t="s">
-        <v>406</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="761" spans="1:2">
       <c r="A761" s="3" t="s">
-        <v>567</v>
+        <v>1445</v>
       </c>
       <c r="B761" s="3" t="s">
-        <v>568</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="762" spans="1:2">
       <c r="A762" s="3" t="s">
-        <v>1455</v>
+        <v>1531</v>
       </c>
       <c r="B762" s="3" t="s">
-        <v>1456</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="763" spans="1:2">
       <c r="A763" s="3" t="s">
-        <v>1457</v>
+        <v>1448</v>
       </c>
       <c r="B763" s="3" t="s">
-        <v>1458</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="764" spans="1:2">
       <c r="A764" s="3" t="s">
-        <v>1459</v>
-      </c>
-      <c r="B764" s="3" t="s">
-        <v>1460</v>
-      </c>
+        <v>1532</v>
+      </c>
+      <c r="B764" s="3"/>
     </row>
     <row r="765" spans="1:2">
       <c r="A765" s="3" t="s">
-        <v>1461</v>
-      </c>
-      <c r="B765" s="3" t="s">
-        <v>682</v>
-      </c>
+        <v>1533</v>
+      </c>
+      <c r="B765" s="3"/>
     </row>
     <row r="766" spans="1:2">
       <c r="A766" s="3" t="s">
-        <v>1462</v>
-      </c>
-      <c r="B766" s="3" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="767" spans="1:2">
-      <c r="A767" s="3" t="s">
-        <v>1463</v>
-      </c>
-      <c r="B767" s="3" t="s">
-        <v>1464</v>
-      </c>
-    </row>
-    <row r="768" spans="1:2">
-      <c r="A768" s="3" t="s">
-        <v>1465</v>
-      </c>
-      <c r="B768" s="3" t="s">
-        <v>1466</v>
-      </c>
-    </row>
-    <row r="769" spans="1:2">
-      <c r="A769" s="3" t="s">
-        <v>1467</v>
-      </c>
-      <c r="B769" s="3" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="770" spans="1:2">
-      <c r="A770" s="3" t="s">
-        <v>1468</v>
-      </c>
-      <c r="B770" s="3" t="s">
-        <v>1468</v>
-      </c>
-    </row>
-    <row r="771" spans="1:2">
-      <c r="A771" s="3" t="s">
-        <v>1469</v>
-      </c>
-      <c r="B771" s="3" t="s">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="772" spans="1:2">
-      <c r="A772" s="3" t="s">
-        <v>1471</v>
-      </c>
-      <c r="B772" s="3" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="773" spans="1:2">
-      <c r="A773" s="3" t="s">
-        <v>1593</v>
-      </c>
-      <c r="B773" s="3" t="s">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="774" spans="1:2">
-      <c r="A774" s="3" t="s">
-        <v>1474</v>
-      </c>
-      <c r="B774" s="3" t="s">
-        <v>1475</v>
-      </c>
-    </row>
-    <row r="775" spans="1:2">
-      <c r="A775" s="3" t="s">
-        <v>1594</v>
-      </c>
-      <c r="B775" s="3"/>
-    </row>
-    <row r="776" spans="1:2">
-      <c r="A776" s="3" t="s">
-        <v>1595</v>
-      </c>
-      <c r="B776" s="3"/>
-    </row>
-    <row r="777" spans="1:2">
-      <c r="A777" s="3" t="s">
-        <v>1596</v>
-      </c>
-      <c r="B777" s="3"/>
+        <v>1534</v>
+      </c>
+      <c r="B766" s="3"/>
+    </row>
+    <row r="767" spans="1:2" s="9" customFormat="1">
+      <c r="A767" s="9" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2" s="9" customFormat="1">
+      <c r="A768" s="9" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2" s="9" customFormat="1">
+      <c r="A769" s="9" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2" s="9" customFormat="1">
+      <c r="A770" s="9" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2" s="9" customFormat="1">
+      <c r="A771" s="9" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2" s="9" customFormat="1">
+      <c r="A772" s="9" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B772" s="9" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2" s="9" customFormat="1">
+      <c r="A773" s="9" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2" s="9" customFormat="1">
+      <c r="A774" s="9" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" s="9" customFormat="1">
+      <c r="A775" s="9" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2" s="9" customFormat="1">
+      <c r="A776" s="9" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B776" s="9" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2" s="9" customFormat="1">
+      <c r="A777" s="9" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B777" s="9" t="s">
+        <v>1454</v>
+      </c>
     </row>
     <row r="778" spans="1:2" s="9" customFormat="1">
       <c r="A778" s="9" t="s">
-        <v>1597</v>
+        <v>1455</v>
+      </c>
+      <c r="B778" s="9" t="s">
+        <v>1456</v>
       </c>
     </row>
     <row r="779" spans="1:2" s="9" customFormat="1">
       <c r="A779" s="9" t="s">
-        <v>1598</v>
+        <v>1457</v>
+      </c>
+      <c r="B779" s="9" t="s">
+        <v>1458</v>
       </c>
     </row>
     <row r="780" spans="1:2" s="9" customFormat="1">
       <c r="A780" s="9" t="s">
-        <v>1599</v>
+        <v>1459</v>
+      </c>
+      <c r="B780" s="9" t="s">
+        <v>1460</v>
       </c>
     </row>
     <row r="781" spans="1:2" s="9" customFormat="1">
       <c r="A781" s="9" t="s">
-        <v>1600</v>
+        <v>1461</v>
+      </c>
+      <c r="B781" s="9" t="s">
+        <v>1462</v>
       </c>
     </row>
     <row r="782" spans="1:2" s="9" customFormat="1">
       <c r="A782" s="9" t="s">
-        <v>1601</v>
+        <v>1463</v>
+      </c>
+      <c r="B782" s="9" t="s">
+        <v>1464</v>
       </c>
     </row>
     <row r="783" spans="1:2" s="9" customFormat="1">
       <c r="A783" s="9" t="s">
-        <v>1602</v>
+        <v>1465</v>
       </c>
       <c r="B783" s="9" t="s">
-        <v>1476</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="784" spans="1:2" s="9" customFormat="1">
       <c r="A784" s="9" t="s">
-        <v>1603</v>
+        <v>1467</v>
+      </c>
+      <c r="B784" s="9" t="s">
+        <v>1468</v>
       </c>
     </row>
     <row r="785" spans="1:2" s="9" customFormat="1">
       <c r="A785" s="9" t="s">
-        <v>1604</v>
+        <v>1469</v>
+      </c>
+      <c r="B785" s="9" t="s">
+        <v>1470</v>
       </c>
     </row>
     <row r="786" spans="1:2" s="9" customFormat="1">
       <c r="A786" s="9" t="s">
-        <v>1605</v>
+        <v>1471</v>
+      </c>
+      <c r="B786" s="9" t="s">
+        <v>1472</v>
       </c>
     </row>
     <row r="787" spans="1:2" s="9" customFormat="1">
       <c r="A787" s="9" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="B787" s="9" t="s">
-        <v>1478</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="788" spans="1:2" s="9" customFormat="1">
       <c r="A788" s="9" t="s">
-        <v>1479</v>
+        <v>1475</v>
       </c>
       <c r="B788" s="9" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="789" spans="1:2" s="9" customFormat="1">
       <c r="A789" s="9" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="B789" s="9" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="790" spans="1:2" s="9" customFormat="1">
       <c r="A790" s="9" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="B790" s="9" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="791" spans="1:2" s="9" customFormat="1">
       <c r="A791" s="9" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="B791" s="9" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="792" spans="1:2" s="9" customFormat="1">
       <c r="A792" s="9" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="B792" s="9" t="s">
-        <v>1488</v>
+        <v>903</v>
       </c>
     </row>
     <row r="793" spans="1:2" s="9" customFormat="1">
       <c r="A793" s="9" t="s">
-        <v>1489</v>
+        <v>1484</v>
       </c>
       <c r="B793" s="9" t="s">
-        <v>1490</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="794" spans="1:2" s="9" customFormat="1">
       <c r="A794" s="9" t="s">
-        <v>1491</v>
+        <v>1486</v>
       </c>
       <c r="B794" s="9" t="s">
-        <v>1492</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="795" spans="1:2" s="9" customFormat="1">
       <c r="A795" s="9" t="s">
-        <v>1493</v>
+        <v>1488</v>
       </c>
       <c r="B795" s="9" t="s">
-        <v>1494</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="796" spans="1:2" s="9" customFormat="1">
       <c r="A796" s="9" t="s">
-        <v>1495</v>
+        <v>1490</v>
       </c>
       <c r="B796" s="9" t="s">
-        <v>1496</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="797" spans="1:2" s="9" customFormat="1">
       <c r="A797" s="9" t="s">
-        <v>1497</v>
+        <v>1492</v>
       </c>
       <c r="B797" s="9" t="s">
-        <v>1498</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="798" spans="1:2" s="9" customFormat="1">
       <c r="A798" s="9" t="s">
-        <v>1499</v>
+        <v>1494</v>
       </c>
       <c r="B798" s="9" t="s">
-        <v>1500</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="799" spans="1:2" s="9" customFormat="1">
       <c r="A799" s="9" t="s">
-        <v>1501</v>
+        <v>1544</v>
       </c>
       <c r="B799" s="9" t="s">
-        <v>1502</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="800" spans="1:2" s="9" customFormat="1">
       <c r="A800" s="9" t="s">
-        <v>1503</v>
+        <v>1497</v>
       </c>
       <c r="B800" s="9" t="s">
-        <v>1504</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="801" spans="1:2" s="9" customFormat="1">
       <c r="A801" s="9" t="s">
-        <v>1505</v>
+        <v>1499</v>
       </c>
       <c r="B801" s="9" t="s">
-        <v>1506</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="802" spans="1:2" s="9" customFormat="1">
       <c r="A802" s="9" t="s">
-        <v>1507</v>
+        <v>1501</v>
       </c>
       <c r="B802" s="9" t="s">
-        <v>1508</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="803" spans="1:2" s="9" customFormat="1">
       <c r="A803" s="9" t="s">
-        <v>1509</v>
+        <v>1503</v>
       </c>
       <c r="B803" s="9" t="s">
-        <v>903</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="804" spans="1:2" s="9" customFormat="1">
       <c r="A804" s="9" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B804" s="9" t="s">
-        <v>1511</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="805" spans="1:2" s="9" customFormat="1">
       <c r="A805" s="9" t="s">
-        <v>1512</v>
+        <v>1554</v>
       </c>
       <c r="B805" s="9" t="s">
-        <v>1513</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="806" spans="1:2" s="9" customFormat="1">
       <c r="A806" s="9" t="s">
-        <v>1514</v>
+        <v>1546</v>
       </c>
       <c r="B806" s="9" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="807" spans="1:2" s="9" customFormat="1">
       <c r="A807" s="9" t="s">
-        <v>1516</v>
+        <v>1550</v>
       </c>
       <c r="B807" s="9" t="s">
-        <v>1517</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="808" spans="1:2" s="9" customFormat="1">
       <c r="A808" s="9" t="s">
-        <v>1518</v>
+        <v>1552</v>
       </c>
       <c r="B808" s="9" t="s">
-        <v>1519</v>
+        <v>165</v>
       </c>
     </row>
     <row r="809" spans="1:2" s="9" customFormat="1">
       <c r="A809" s="9" t="s">
-        <v>1520</v>
+        <v>1547</v>
       </c>
       <c r="B809" s="9" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="810" spans="1:2" s="9" customFormat="1">
-      <c r="A810" s="9" t="s">
-        <v>1606</v>
-      </c>
-      <c r="B810" s="9" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="811" spans="1:2" s="9" customFormat="1">
-      <c r="A811" s="9" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B811" s="9" t="s">
-        <v>1524</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" s="9" customFormat="1">
-      <c r="A812" s="9" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B812" s="9" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="813" spans="1:2" s="9" customFormat="1">
-      <c r="A813" s="9" t="s">
-        <v>1527</v>
-      </c>
-      <c r="B813" s="9" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="814" spans="1:2" s="9" customFormat="1">
-      <c r="A814" s="9" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B814" s="9" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="815" spans="1:2" s="9" customFormat="1">
-      <c r="A815" s="9" t="s">
-        <v>1537</v>
-      </c>
-      <c r="B815" s="9" t="s">
-        <v>1607</v>
-      </c>
-    </row>
-    <row r="816" spans="1:2" s="9" customFormat="1">
-      <c r="A816" s="9" t="s">
-        <v>1619</v>
-      </c>
-      <c r="B816" s="9" t="s">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" s="9" customFormat="1">
-      <c r="A817" s="9" t="s">
-        <v>1608</v>
-      </c>
-      <c r="B817" s="9" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="818" spans="1:2" s="9" customFormat="1">
-      <c r="A818" s="9" t="s">
-        <v>1615</v>
-      </c>
-      <c r="B818" s="9" t="s">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" s="9" customFormat="1">
-      <c r="A819" s="9" t="s">
-        <v>1617</v>
-      </c>
-      <c r="B819" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="820" spans="1:2" s="9" customFormat="1">
-      <c r="A820" s="9" t="s">
-        <v>1609</v>
-      </c>
-      <c r="B820" s="9" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="821" spans="1:2" s="9" customFormat="1">
-      <c r="A821" s="9" t="s">
-        <v>1611</v>
-      </c>
-      <c r="B821" s="9" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" s="9" customFormat="1">
-      <c r="A822" s="9" t="s">
-        <v>1546</v>
-      </c>
-      <c r="B822" s="9" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="823" spans="1:2" s="9" customFormat="1">
-      <c r="A823" s="9" t="s">
-        <v>1547</v>
-      </c>
-      <c r="B823" s="9" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" s="9" customFormat="1">
-      <c r="A824" s="9" t="s">
         <v>1548</v>
       </c>
-      <c r="B824" s="9" t="s">
-        <v>1551</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" s="9" customFormat="1">
-      <c r="A825" s="9" t="s">
-        <v>1612</v>
-      </c>
-      <c r="B825" s="9" t="s">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="826" spans="1:2" s="9" customFormat="1">
-      <c r="A826" s="9" t="s">
-        <v>1387</v>
-      </c>
-      <c r="B826" s="9" t="s">
-        <v>1388</v>
-      </c>
+    </row>
+    <row r="810" spans="1:2" s="9" customFormat="1"/>
+    <row r="811" spans="1:2" s="9" customFormat="1"/>
+    <row r="812" spans="1:2" s="9" customFormat="1"/>
+    <row r="813" spans="1:2" s="9" customFormat="1"/>
+    <row r="814" spans="1:2" s="9" customFormat="1"/>
+    <row r="815" spans="1:2" s="9" customFormat="1"/>
+    <row r="816" spans="1:2">
+      <c r="A816" s="6"/>
+      <c r="B816" s="10"/>
+    </row>
+    <row r="817" spans="1:2">
+      <c r="A817" s="6"/>
+      <c r="B817" s="6"/>
+    </row>
+    <row r="818" spans="1:2">
+      <c r="A818" s="6"/>
+      <c r="B818" s="6"/>
+    </row>
+    <row r="820" spans="1:2">
+      <c r="A820" s="3"/>
+      <c r="B820" s="7"/>
+    </row>
+    <row r="821" spans="1:2">
+      <c r="A821" s="3"/>
+      <c r="B821" s="7"/>
+    </row>
+    <row r="822" spans="1:2">
+      <c r="A822" s="3"/>
+      <c r="B822" s="7"/>
+    </row>
+    <row r="823" spans="1:2">
+      <c r="A823" s="3"/>
+      <c r="B823" s="7"/>
+    </row>
+    <row r="824" spans="1:2">
+      <c r="A824" s="2"/>
+      <c r="B824" s="7"/>
+    </row>
+    <row r="825" spans="1:2">
+      <c r="A825" s="3"/>
+      <c r="B825" s="7"/>
+    </row>
+    <row r="826" spans="1:2">
+      <c r="A826" s="3"/>
+      <c r="B826" s="5"/>
     </row>
     <row r="827" spans="1:2">
-      <c r="A827" s="6" t="s">
-        <v>1552</v>
-      </c>
-      <c r="B827" s="10" t="s">
-        <v>1553</v>
-      </c>
+      <c r="A827" s="3"/>
+      <c r="B827" s="7"/>
     </row>
     <row r="828" spans="1:2">
-      <c r="A828" s="6" t="s">
-        <v>1381</v>
-      </c>
-      <c r="B828" s="6" t="s">
-        <v>1382</v>
-      </c>
+      <c r="A828" s="3"/>
+      <c r="B828" s="7"/>
     </row>
     <row r="829" spans="1:2">
-      <c r="A829" s="6" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B829" s="6" t="s">
-        <v>1572</v>
-      </c>
+      <c r="A829" s="3"/>
+      <c r="B829" s="7"/>
     </row>
     <row r="830" spans="1:2">
-      <c r="A830" t="s">
-        <v>1557</v>
-      </c>
-      <c r="B830" t="s">
-        <v>1573</v>
-      </c>
+      <c r="A830" s="3"/>
+      <c r="B830" s="7"/>
     </row>
     <row r="831" spans="1:2">
-      <c r="A831" s="3" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B831" s="7" t="s">
-        <v>1558</v>
-      </c>
+      <c r="A831" s="6"/>
+      <c r="B831" s="6"/>
     </row>
     <row r="832" spans="1:2">
-      <c r="A832" s="3" t="s">
-        <v>1556</v>
-      </c>
-      <c r="B832" s="7" t="s">
-        <v>1574</v>
-      </c>
+      <c r="A832" s="6"/>
+      <c r="B832" s="5"/>
     </row>
     <row r="833" spans="1:2">
-      <c r="A833" s="3" t="s">
-        <v>1535</v>
-      </c>
-      <c r="B833" s="7" t="s">
-        <v>1536</v>
-      </c>
+      <c r="A833" s="2"/>
+      <c r="B833" s="7"/>
     </row>
     <row r="834" spans="1:2">
-      <c r="A834" s="3" t="s">
-        <v>1559</v>
-      </c>
-      <c r="B834" s="7" t="s">
-        <v>1560</v>
-      </c>
+      <c r="A834" s="2"/>
+      <c r="B834" s="7"/>
     </row>
     <row r="835" spans="1:2">
-      <c r="A835" s="2" t="s">
-        <v>1561</v>
-      </c>
-      <c r="B835" s="7" t="s">
-        <v>1564</v>
-      </c>
+      <c r="A835" s="2"/>
+      <c r="B835" s="7"/>
     </row>
     <row r="836" spans="1:2">
-      <c r="A836" s="3" t="s">
-        <v>1562</v>
-      </c>
-      <c r="B836" s="7" t="s">
-        <v>1565</v>
-      </c>
+      <c r="A836" s="2"/>
+      <c r="B836" s="7"/>
     </row>
     <row r="837" spans="1:2">
-      <c r="A837" s="3" t="s">
-        <v>1563</v>
-      </c>
-      <c r="B837" s="5" t="s">
-        <v>1566</v>
-      </c>
+      <c r="A837" s="2"/>
+      <c r="B837" s="5"/>
     </row>
     <row r="838" spans="1:2">
-      <c r="A838" s="3" t="s">
-        <v>1391</v>
-      </c>
-      <c r="B838" s="7" t="s">
-        <v>1392</v>
-      </c>
+      <c r="A838" s="2"/>
+      <c r="B838" s="5"/>
     </row>
     <row r="839" spans="1:2">
-      <c r="A839" s="3" t="s">
-        <v>1567</v>
-      </c>
-      <c r="B839" s="7" t="s">
-        <v>1568</v>
-      </c>
+      <c r="A839" s="2"/>
+      <c r="B839" s="5"/>
     </row>
     <row r="840" spans="1:2">
-      <c r="A840" s="3" t="s">
-        <v>1389</v>
-      </c>
-      <c r="B840" s="7" t="s">
-        <v>1390</v>
-      </c>
+      <c r="A840" s="2"/>
+      <c r="B840" s="5"/>
     </row>
     <row r="841" spans="1:2">
-      <c r="A841" s="3" t="s">
-        <v>1570</v>
-      </c>
-      <c r="B841" s="7" t="s">
-        <v>1571</v>
-      </c>
+      <c r="B841" s="7"/>
     </row>
     <row r="842" spans="1:2">
-      <c r="A842" s="6" t="s">
-        <v>1569</v>
-      </c>
-      <c r="B842" s="6" t="s">
-        <v>1624</v>
-      </c>
+      <c r="A842" s="2"/>
+      <c r="B842" s="5"/>
     </row>
     <row r="843" spans="1:2">
-      <c r="A843" s="6" t="s">
-        <v>1626</v>
-      </c>
-      <c r="B843" s="5" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="844" spans="1:2">
-      <c r="A844" s="2" t="s">
-        <v>1415</v>
-      </c>
-      <c r="B844" s="7" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="845" spans="1:2">
-      <c r="A845" s="2" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B845" s="7" t="s">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="846" spans="1:2">
-      <c r="A846" s="2" t="s">
-        <v>1576</v>
-      </c>
-      <c r="B846" s="7" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="847" spans="1:2">
-      <c r="A847" s="2"/>
-      <c r="B847" s="7"/>
-    </row>
-    <row r="848" spans="1:2">
-      <c r="A848" s="2"/>
-      <c r="B848" s="5"/>
-    </row>
-    <row r="849" spans="1:2">
-      <c r="A849" s="2"/>
-      <c r="B849" s="5"/>
-    </row>
-    <row r="850" spans="1:2">
-      <c r="A850" s="2"/>
-      <c r="B850" s="5"/>
-    </row>
-    <row r="851" spans="1:2">
-      <c r="A851" s="2"/>
-      <c r="B851" s="5"/>
-    </row>
-    <row r="852" spans="1:2">
-      <c r="B852" s="7"/>
-    </row>
-    <row r="853" spans="1:2">
-      <c r="A853" s="2"/>
-      <c r="B853" s="5"/>
-    </row>
-    <row r="854" spans="1:2">
-      <c r="A854" s="2"/>
-      <c r="B854" s="5"/>
+      <c r="A843" s="2"/>
+      <c r="B843" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>